<commit_message>
fix error in flexible cola function
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -1311,7 +1311,7 @@
   <dimension ref="A3:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,7 +1353,7 @@
         <v>2000</v>
       </c>
       <c r="C4">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D4">
         <v>6</v>

</xml_diff>

<commit_message>
5-year min amort period
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="111">
   <si>
     <t>runname</t>
   </si>
@@ -350,6 +350,12 @@
   </si>
   <si>
     <t>m.min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">closed </t>
+  </si>
+  <si>
+    <t>MISERS assumption met; min m = 5</t>
   </si>
 </sst>
 </file>
@@ -1033,10 +1039,10 @@
   <dimension ref="A4:AS28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="P5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Y33" sqref="Y33"/>
+      <selection pane="bottomRight" activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2012,16 +2018,16 @@
         <v>107</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="E14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>54</v>
@@ -2060,7 +2066,7 @@
         <v>56</v>
       </c>
       <c r="R14" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="S14">
         <v>20</v>
@@ -2078,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="X14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Y14">
         <v>0.04</v>

</xml_diff>